<commit_message>
Se añade pmdarima y se actualizan los datos
</commit_message>
<xml_diff>
--- a/df_st_test.xlsx
+++ b/df_st_test.xlsx
@@ -497,1908 +497,1908 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>presMax</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>horaPresMax</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>presMin</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>horaPresMin</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>hrMedia</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>hrMax</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>horaHrMax</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>hrMin</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>horaHrMin</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>presMax</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>horaPresMax</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>presMin</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>horaPresMin</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45721</v>
+        <v>45754</v>
       </c>
       <c r="B2" t="n">
-        <v>10.8</v>
+        <v>15.8</v>
       </c>
       <c r="C2" t="n">
-        <v>4.4</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>8.5</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E2" t="n">
-        <v>6</v>
+        <v>6.3</v>
       </c>
       <c r="F2" t="n">
-        <v>13</v>
+        <v>22.8</v>
       </c>
       <c r="G2" t="n">
-        <v>13.5</v>
+        <v>14.2</v>
       </c>
       <c r="H2" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="I2" t="n">
-        <v>2.8</v>
+        <v>1.1</v>
       </c>
       <c r="J2" t="n">
-        <v>8.1</v>
+        <v>5.3</v>
       </c>
       <c r="K2" t="n">
-        <v>8.199999999999999</v>
+        <v>14</v>
       </c>
       <c r="L2" t="n">
-        <v>88</v>
+        <v>941.9</v>
       </c>
       <c r="M2" t="n">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="N2" t="n">
-        <v>22.4</v>
+        <v>938.2</v>
       </c>
       <c r="O2" t="n">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="P2" t="n">
-        <v>16.3</v>
+        <v>56</v>
       </c>
       <c r="Q2" t="n">
-        <v>939.3</v>
+        <v>94</v>
       </c>
       <c r="R2" t="n">
-        <v>22</v>
+        <v>3.3</v>
       </c>
       <c r="S2" t="n">
-        <v>936.7</v>
+        <v>30</v>
       </c>
       <c r="T2" t="n">
-        <v>5</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45722</v>
+        <v>45755</v>
       </c>
       <c r="B3" t="n">
-        <v>10.8</v>
+        <v>18</v>
       </c>
       <c r="C3" t="n">
-        <v>16.1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>8.5</v>
+        <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
-        <v>13.2</v>
+        <v>24.9</v>
       </c>
       <c r="G3" t="n">
-        <v>13.2</v>
+        <v>14.2</v>
       </c>
       <c r="H3" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="I3" t="n">
-        <v>2.2</v>
+        <v>1.4</v>
       </c>
       <c r="J3" t="n">
-        <v>8.9</v>
+        <v>6.7</v>
       </c>
       <c r="K3" t="n">
-        <v>12.1</v>
+        <v>12.3</v>
       </c>
       <c r="L3" t="n">
-        <v>92</v>
+        <v>943.7</v>
       </c>
       <c r="M3" t="n">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="N3" t="n">
-        <v>23.3</v>
+        <v>940.2</v>
       </c>
       <c r="O3" t="n">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="P3" t="n">
-        <v>16.4</v>
+        <v>45</v>
       </c>
       <c r="Q3" t="n">
-        <v>937.2</v>
+        <v>80</v>
       </c>
       <c r="R3" t="n">
-        <v>23</v>
+        <v>4.1</v>
       </c>
       <c r="S3" t="n">
-        <v>934.5</v>
+        <v>28</v>
       </c>
       <c r="T3" t="n">
-        <v>6</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45723</v>
+        <v>45756</v>
       </c>
       <c r="B4" t="n">
-        <v>10.4</v>
+        <v>18.6</v>
       </c>
       <c r="C4" t="n">
-        <v>21.9</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>8.699999999999999</v>
+        <v>12.6</v>
       </c>
       <c r="E4" t="n">
-        <v>3.3</v>
+        <v>6.5</v>
       </c>
       <c r="F4" t="n">
-        <v>12</v>
+        <v>24.6</v>
       </c>
       <c r="G4" t="n">
-        <v>14.2</v>
+        <v>15.1</v>
       </c>
       <c r="H4" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="I4" t="n">
-        <v>2.5</v>
+        <v>2.2</v>
       </c>
       <c r="J4" t="n">
-        <v>9.199999999999999</v>
+        <v>6.7</v>
       </c>
       <c r="K4" t="n">
-        <v>15.4</v>
+        <v>4</v>
       </c>
       <c r="L4" t="n">
-        <v>96</v>
+        <v>941.6</v>
       </c>
       <c r="M4" t="n">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="N4" t="n">
-        <v>7.4</v>
+        <v>936.9</v>
       </c>
       <c r="O4" t="n">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="P4" t="n">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="Q4" t="n">
-        <v>936.7</v>
+        <v>61</v>
       </c>
       <c r="R4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S4" t="n">
-        <v>928.8</v>
+        <v>25</v>
       </c>
       <c r="T4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45724</v>
+        <v>45757</v>
       </c>
       <c r="B5" t="n">
-        <v>8.4</v>
+        <v>18.2</v>
       </c>
       <c r="C5" t="n">
-        <v>13.8</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>5.7</v>
+        <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>23.59</v>
+        <v>5.2</v>
       </c>
       <c r="F5" t="n">
-        <v>11.2</v>
+        <v>23.5</v>
       </c>
       <c r="G5" t="n">
-        <v>13.1</v>
+        <v>13.4</v>
       </c>
       <c r="H5" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I5" t="n">
-        <v>4.2</v>
+        <v>3.6</v>
       </c>
       <c r="J5" t="n">
-        <v>16.7</v>
+        <v>10.6</v>
       </c>
       <c r="K5" t="n">
-        <v>12.5</v>
+        <v>17</v>
       </c>
       <c r="L5" t="n">
-        <v>92</v>
+        <v>941</v>
       </c>
       <c r="M5" t="n">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N5" t="n">
-        <v>1</v>
+        <v>937.2</v>
       </c>
       <c r="O5" t="n">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="P5" t="n">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="Q5" t="n">
-        <v>929.3</v>
+        <v>68</v>
       </c>
       <c r="R5" t="n">
-        <v>0</v>
+        <v>5.1</v>
       </c>
       <c r="S5" t="n">
-        <v>919</v>
+        <v>34</v>
       </c>
       <c r="T5" t="n">
-        <v>17</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45725</v>
+        <v>45758</v>
       </c>
       <c r="B6" t="n">
-        <v>7.2</v>
+        <v>13.2</v>
       </c>
       <c r="C6" t="n">
-        <v>3.6</v>
+        <v>11.3</v>
       </c>
       <c r="D6" t="n">
-        <v>4.1</v>
+        <v>10.7</v>
       </c>
       <c r="E6" t="n">
-        <v>6.3</v>
+        <v>11.1</v>
       </c>
       <c r="F6" t="n">
-        <v>10.3</v>
+        <v>15.7</v>
       </c>
       <c r="G6" t="n">
-        <v>14</v>
+        <v>15.3</v>
       </c>
       <c r="H6" t="n">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="I6" t="n">
-        <v>2.2</v>
+        <v>2.5</v>
       </c>
       <c r="J6" t="n">
-        <v>11.1</v>
+        <v>8.1</v>
       </c>
       <c r="K6" t="n">
-        <v>11.2</v>
+        <v>15.3</v>
       </c>
       <c r="L6" t="n">
-        <v>86</v>
+        <v>940.7</v>
       </c>
       <c r="M6" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>3.3</v>
+        <v>933.6</v>
       </c>
       <c r="O6" t="n">
-        <v>70</v>
+        <v>17</v>
       </c>
       <c r="P6" t="n">
-        <v>13.4</v>
+        <v>75</v>
       </c>
       <c r="Q6" t="n">
-        <v>923.6</v>
+        <v>96</v>
       </c>
       <c r="R6" t="n">
-        <v>22</v>
+        <v>23.59</v>
       </c>
       <c r="S6" t="n">
-        <v>921.1</v>
+        <v>62</v>
       </c>
       <c r="T6" t="n">
-        <v>16</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45726</v>
+        <v>45759</v>
       </c>
       <c r="B7" t="n">
-        <v>8.6</v>
+        <v>13.8</v>
       </c>
       <c r="C7" t="n">
-        <v>23.5</v>
+        <v>4.5</v>
       </c>
       <c r="D7" t="n">
-        <v>5.8</v>
+        <v>10.8</v>
       </c>
       <c r="E7" t="n">
-        <v>6.05</v>
+        <v>4.3</v>
       </c>
       <c r="F7" t="n">
-        <v>11.5</v>
+        <v>16.7</v>
       </c>
       <c r="G7" t="n">
-        <v>15</v>
+        <v>12.2</v>
       </c>
       <c r="H7" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I7" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="J7" t="n">
-        <v>3.1</v>
+        <v>6.4</v>
       </c>
       <c r="K7" t="n">
-        <v>7.5</v>
+        <v>17</v>
       </c>
       <c r="L7" t="n">
-        <v>89</v>
+        <v>935</v>
       </c>
       <c r="M7" t="n">
-        <v>89</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>8</v>
+        <v>931.5</v>
       </c>
       <c r="O7" t="n">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="P7" t="n">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="Q7" t="n">
-        <v>942.7</v>
+        <v>98</v>
       </c>
       <c r="R7" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="S7" t="n">
-        <v>939.8</v>
+        <v>75</v>
       </c>
       <c r="T7" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45727</v>
+        <v>45760</v>
       </c>
       <c r="B8" t="n">
-        <v>8.4</v>
+        <v>14.8</v>
       </c>
       <c r="C8" t="n">
-        <v>7.5</v>
+        <v>3.6</v>
       </c>
       <c r="D8" t="n">
-        <v>6.2</v>
+        <v>11.7</v>
       </c>
       <c r="E8" t="n">
-        <v>23.59</v>
+        <v>5.5</v>
       </c>
       <c r="F8" t="n">
-        <v>10.6</v>
+        <v>17.9</v>
       </c>
       <c r="G8" t="n">
-        <v>16.4</v>
+        <v>12.3</v>
       </c>
       <c r="H8" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="I8" t="n">
-        <v>2.2</v>
+        <v>1.1</v>
       </c>
       <c r="J8" t="n">
-        <v>10.3</v>
+        <v>5.3</v>
       </c>
       <c r="K8" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="L8" t="n">
+        <v>933.6</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>931.1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>17</v>
+      </c>
+      <c r="P8" t="n">
+        <v>85</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>99</v>
+      </c>
+      <c r="R8" t="n">
+        <v>2</v>
+      </c>
+      <c r="S8" t="n">
+        <v>67</v>
+      </c>
+      <c r="T8" t="n">
         <v>13.1</v>
-      </c>
-      <c r="L8" t="n">
-        <v>77</v>
-      </c>
-      <c r="M8" t="n">
-        <v>90</v>
-      </c>
-      <c r="N8" t="n">
-        <v>4</v>
-      </c>
-      <c r="O8" t="n">
-        <v>60</v>
-      </c>
-      <c r="P8" t="n">
-        <v>14</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>925.8</v>
-      </c>
-      <c r="R8" t="n">
-        <v>24</v>
-      </c>
-      <c r="S8" t="n">
-        <v>921.6</v>
-      </c>
-      <c r="T8" t="n">
-        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45728</v>
+        <v>45761</v>
       </c>
       <c r="B9" t="n">
-        <v>8.5</v>
+        <v>13.3</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>4.9</v>
       </c>
       <c r="D9" t="n">
-        <v>4.2</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>21.1</v>
       </c>
       <c r="F9" t="n">
-        <v>12.8</v>
+        <v>16.9</v>
       </c>
       <c r="G9" t="n">
-        <v>13.2</v>
+        <v>14</v>
       </c>
       <c r="H9" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="I9" t="n">
-        <v>2.5</v>
+        <v>3.6</v>
       </c>
       <c r="J9" t="n">
-        <v>10</v>
+        <v>11.7</v>
       </c>
       <c r="K9" t="n">
-        <v>15.1</v>
+        <v>13</v>
       </c>
       <c r="L9" t="n">
-        <v>60</v>
+        <v>931.8</v>
       </c>
       <c r="M9" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="N9" t="n">
-        <v>7</v>
+        <v>926.8</v>
       </c>
       <c r="O9" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="P9" t="n">
-        <v>14.1</v>
+        <v>67</v>
       </c>
       <c r="Q9" t="n">
-        <v>928.1</v>
+        <v>95</v>
       </c>
       <c r="R9" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="S9" t="n">
-        <v>923.5</v>
+        <v>46</v>
       </c>
       <c r="T9" t="n">
-        <v>24</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45729</v>
+        <v>45762</v>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="C10" t="n">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>4.3</v>
+        <v>6.2</v>
       </c>
       <c r="E10" t="n">
-        <v>23.5</v>
+        <v>23.59</v>
       </c>
       <c r="F10" t="n">
-        <v>11.6</v>
+        <v>11.5</v>
       </c>
       <c r="G10" t="n">
-        <v>15</v>
+        <v>11.4</v>
       </c>
       <c r="H10" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="I10" t="n">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
       <c r="J10" t="n">
-        <v>10.3</v>
+        <v>11.4</v>
       </c>
       <c r="K10" t="n">
-        <v>23.1</v>
+        <v>19.1</v>
       </c>
       <c r="L10" t="n">
-        <v>89</v>
+        <v>932.6</v>
       </c>
       <c r="M10" t="n">
+        <v>24</v>
+      </c>
+      <c r="N10" t="n">
+        <v>926.2</v>
+      </c>
+      <c r="O10" t="n">
+        <v>3</v>
+      </c>
+      <c r="P10" t="n">
+        <v>71</v>
+      </c>
+      <c r="Q10" t="n">
         <v>98</v>
       </c>
-      <c r="N10" t="n">
-        <v>18.4</v>
-      </c>
-      <c r="O10" t="n">
-        <v>63</v>
-      </c>
-      <c r="P10" t="n">
-        <v>14.3</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>923.5</v>
-      </c>
       <c r="R10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S10" t="n">
-        <v>915.9</v>
+        <v>51</v>
       </c>
       <c r="T10" t="n">
-        <v>15</v>
+        <v>18.1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45730</v>
+        <v>45763</v>
       </c>
       <c r="B11" t="n">
-        <v>7.2</v>
+        <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="D11" t="n">
-        <v>4.1</v>
+        <v>5.2</v>
       </c>
       <c r="E11" t="n">
-        <v>23.5</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
-        <v>10.4</v>
+        <v>12.9</v>
       </c>
       <c r="G11" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="I11" t="n">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="J11" t="n">
-        <v>12.2</v>
+        <v>10.3</v>
       </c>
       <c r="K11" t="n">
-        <v>9.1</v>
+        <v>13.5</v>
       </c>
       <c r="L11" t="n">
-        <v>57</v>
+        <v>937.2</v>
       </c>
       <c r="M11" t="n">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="N11" t="n">
-        <v>0</v>
+        <v>932.4</v>
       </c>
       <c r="O11" t="n">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="P11" t="n">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="Q11" t="n">
-        <v>929.6</v>
+        <v>99</v>
       </c>
       <c r="R11" t="n">
-        <v>24</v>
+        <v>0.2</v>
       </c>
       <c r="S11" t="n">
-        <v>919.3</v>
+        <v>45</v>
       </c>
       <c r="T11" t="n">
-        <v>4</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45731</v>
+        <v>45764</v>
       </c>
       <c r="B12" t="n">
-        <v>5.8</v>
+        <v>12.8</v>
       </c>
       <c r="C12" t="n">
-        <v>6.7</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>1.1</v>
+        <v>6.2</v>
       </c>
       <c r="E12" t="n">
-        <v>6</v>
+        <v>6.3</v>
       </c>
       <c r="F12" t="n">
-        <v>10.6</v>
+        <v>19.3</v>
       </c>
       <c r="G12" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="H12" t="n">
         <v>14</v>
       </c>
-      <c r="H12" t="n">
-        <v>3</v>
-      </c>
       <c r="I12" t="n">
-        <v>1.9</v>
+        <v>3.1</v>
       </c>
       <c r="J12" t="n">
-        <v>6.7</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="K12" t="n">
-        <v>0.1</v>
+        <v>7.5</v>
       </c>
       <c r="L12" t="n">
-        <v>60</v>
+        <v>939.2</v>
       </c>
       <c r="M12" t="n">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="N12" t="n">
-        <v>5.2</v>
+        <v>936.7</v>
       </c>
       <c r="O12" t="n">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="P12" t="n">
-        <v>13.5</v>
+        <v>53</v>
       </c>
       <c r="Q12" t="n">
-        <v>936.1</v>
+        <v>99</v>
       </c>
       <c r="R12" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="S12" t="n">
-        <v>929.6</v>
+        <v>34</v>
       </c>
       <c r="T12" t="n">
-        <v>0</v>
+        <v>12.4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45732</v>
+        <v>45765</v>
       </c>
       <c r="B13" t="n">
-        <v>7.8</v>
+        <v>14.2</v>
       </c>
       <c r="C13" t="n">
-        <v>0.4</v>
+        <v>12.7</v>
       </c>
       <c r="D13" t="n">
-        <v>4.1</v>
+        <v>9.4</v>
       </c>
       <c r="E13" t="n">
-        <v>7.5</v>
+        <v>5.4</v>
       </c>
       <c r="F13" t="n">
-        <v>11.6</v>
+        <v>18.9</v>
       </c>
       <c r="G13" t="n">
-        <v>15.3</v>
+        <v>14</v>
       </c>
       <c r="H13" t="n">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="I13" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="J13" t="n">
-        <v>7.2</v>
+        <v>15.8</v>
       </c>
       <c r="K13" t="n">
-        <v>9.5</v>
+        <v>17.3</v>
       </c>
       <c r="L13" t="n">
-        <v>69</v>
+        <v>939</v>
       </c>
       <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>929.7</v>
+      </c>
+      <c r="O13" t="n">
+        <v>24</v>
+      </c>
+      <c r="P13" t="n">
+        <v>84</v>
+      </c>
+      <c r="Q13" t="n">
         <v>98</v>
       </c>
-      <c r="N13" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="O13" t="n">
-        <v>44</v>
-      </c>
-      <c r="P13" t="n">
-        <v>18</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>938.2</v>
-      </c>
       <c r="R13" t="n">
-        <v>20</v>
+        <v>19.4</v>
       </c>
       <c r="S13" t="n">
-        <v>934.3</v>
+        <v>54</v>
       </c>
       <c r="T13" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45733</v>
+        <v>45766</v>
       </c>
       <c r="B14" t="n">
-        <v>6.8</v>
+        <v>9.5</v>
       </c>
       <c r="C14" t="n">
-        <v>16.7</v>
+        <v>4.8</v>
       </c>
       <c r="D14" t="n">
-        <v>4.2</v>
+        <v>5.8</v>
       </c>
       <c r="E14" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F14" t="n">
-        <v>9.4</v>
+        <v>13.2</v>
       </c>
       <c r="G14" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H14" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I14" t="n">
-        <v>3.1</v>
+        <v>3.9</v>
       </c>
       <c r="J14" t="n">
-        <v>10.6</v>
+        <v>13.3</v>
       </c>
       <c r="K14" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L14" t="n">
-        <v>88</v>
+        <v>930.4</v>
       </c>
       <c r="M14" t="n">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N14" t="n">
-        <v>23.59</v>
+        <v>927</v>
       </c>
       <c r="O14" t="n">
-        <v>58</v>
+        <v>4</v>
       </c>
       <c r="P14" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="Q14" t="n">
-        <v>937.8</v>
+        <v>98</v>
       </c>
       <c r="R14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S14" t="n">
-        <v>932.5</v>
+        <v>47</v>
       </c>
       <c r="T14" t="n">
-        <v>18</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45734</v>
+        <v>45767</v>
       </c>
       <c r="B15" t="n">
-        <v>8.800000000000001</v>
+        <v>11.2</v>
       </c>
       <c r="C15" t="n">
-        <v>20.9</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>6.2</v>
       </c>
       <c r="E15" t="n">
-        <v>23.59</v>
+        <v>5.1</v>
       </c>
       <c r="F15" t="n">
-        <v>11.4</v>
+        <v>16.2</v>
       </c>
       <c r="G15" t="n">
-        <v>16</v>
+        <v>14.2</v>
       </c>
       <c r="H15" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I15" t="n">
-        <v>2.8</v>
+        <v>2.2</v>
       </c>
       <c r="J15" t="n">
-        <v>10.8</v>
+        <v>10</v>
       </c>
       <c r="K15" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="L15" t="n">
-        <v>76</v>
+        <v>937.1</v>
       </c>
       <c r="M15" t="n">
-        <v>87</v>
+        <v>24</v>
       </c>
       <c r="N15" t="n">
-        <v>8.4</v>
+        <v>929.2</v>
       </c>
       <c r="O15" t="n">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="P15" t="n">
-        <v>14.4</v>
+        <v>63</v>
       </c>
       <c r="Q15" t="n">
-        <v>938.3</v>
+        <v>96</v>
       </c>
       <c r="R15" t="n">
-        <v>24</v>
+        <v>4.2</v>
       </c>
       <c r="S15" t="n">
-        <v>931.8</v>
+        <v>39</v>
       </c>
       <c r="T15" t="n">
-        <v>14</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45735</v>
+        <v>45768</v>
       </c>
       <c r="B16" t="n">
-        <v>12.4</v>
+        <v>13.2</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D16" t="n">
-        <v>8.1</v>
+        <v>7.5</v>
       </c>
       <c r="E16" t="n">
-        <v>7</v>
+        <v>5.5</v>
       </c>
       <c r="F16" t="n">
-        <v>16.6</v>
+        <v>19</v>
       </c>
       <c r="G16" t="n">
-        <v>16</v>
+        <v>14.4</v>
       </c>
       <c r="H16" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I16" t="n">
-        <v>3.3</v>
+        <v>1.9</v>
       </c>
       <c r="J16" t="n">
-        <v>13.1</v>
+        <v>7.5</v>
       </c>
       <c r="K16" t="n">
-        <v>21.1</v>
+        <v>0.1</v>
       </c>
       <c r="L16" t="n">
-        <v>74</v>
+        <v>939.8</v>
       </c>
       <c r="M16" t="n">
-        <v>99</v>
+        <v>22</v>
       </c>
       <c r="N16" t="n">
-        <v>0</v>
+        <v>937</v>
       </c>
       <c r="O16" t="n">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="P16" t="n">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="Q16" t="n">
-        <v>940.1</v>
+        <v>94</v>
       </c>
       <c r="R16" t="n">
-        <v>10</v>
+        <v>23.5</v>
       </c>
       <c r="S16" t="n">
-        <v>935.9</v>
+        <v>41</v>
       </c>
       <c r="T16" t="n">
-        <v>18</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45736</v>
+        <v>45769</v>
       </c>
       <c r="B17" t="n">
-        <v>12.7</v>
+        <v>14.8</v>
       </c>
       <c r="C17" t="n">
-        <v>27.6</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>9.300000000000001</v>
+        <v>10.6</v>
       </c>
       <c r="E17" t="n">
-        <v>22.3</v>
+        <v>5</v>
       </c>
       <c r="F17" t="n">
-        <v>16.1</v>
+        <v>18.9</v>
       </c>
       <c r="G17" t="n">
-        <v>16.5</v>
+        <v>16.2</v>
       </c>
       <c r="H17" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="I17" t="n">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="J17" t="n">
-        <v>11.7</v>
+        <v>8.1</v>
       </c>
       <c r="K17" t="n">
-        <v>2.3</v>
+        <v>19.4</v>
       </c>
       <c r="L17" t="n">
-        <v>79</v>
+        <v>944.5</v>
       </c>
       <c r="M17" t="n">
-        <v>99</v>
+        <v>24</v>
       </c>
       <c r="N17" t="n">
-        <v>11</v>
+        <v>938.7</v>
       </c>
       <c r="O17" t="n">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="P17" t="n">
-        <v>16.1</v>
+        <v>63</v>
       </c>
       <c r="Q17" t="n">
-        <v>937.8</v>
+        <v>98</v>
       </c>
       <c r="R17" t="n">
-        <v>24</v>
+        <v>4.5</v>
       </c>
       <c r="S17" t="n">
-        <v>931.8</v>
+        <v>41</v>
       </c>
       <c r="T17" t="n">
-        <v>24</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45737</v>
+        <v>45770</v>
       </c>
       <c r="B18" t="n">
+        <v>15.5</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="E18" t="n">
+        <v>6</v>
+      </c>
+      <c r="F18" t="n">
+        <v>22.4</v>
+      </c>
+      <c r="G18" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="H18" t="n">
+        <v>26</v>
+      </c>
+      <c r="I18" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="J18" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="K18" t="n">
+        <v>14.1</v>
+      </c>
+      <c r="L18" t="n">
+        <v>945.7</v>
+      </c>
+      <c r="M18" t="n">
         <v>9</v>
       </c>
-      <c r="C18" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="D18" t="n">
+      <c r="N18" t="n">
+        <v>942</v>
+      </c>
+      <c r="O18" t="n">
+        <v>17</v>
+      </c>
+      <c r="P18" t="n">
+        <v>52</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>84</v>
+      </c>
+      <c r="R18" t="n">
         <v>6.3</v>
       </c>
-      <c r="E18" t="n">
-        <v>23.59</v>
-      </c>
-      <c r="F18" t="n">
-        <v>11.8</v>
-      </c>
-      <c r="G18" t="n">
-        <v>14.1</v>
-      </c>
-      <c r="H18" t="n">
-        <v>24</v>
-      </c>
-      <c r="I18" t="n">
-        <v>3.6</v>
-      </c>
-      <c r="J18" t="n">
-        <v>16.9</v>
-      </c>
-      <c r="K18" t="n">
-        <v>22.1</v>
-      </c>
-      <c r="L18" t="n">
-        <v>87</v>
-      </c>
-      <c r="M18" t="n">
-        <v>98</v>
-      </c>
-      <c r="N18" t="n">
-        <v>23</v>
-      </c>
-      <c r="O18" t="n">
-        <v>65</v>
-      </c>
-      <c r="P18" t="n">
-        <v>11.3</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>932.5</v>
-      </c>
-      <c r="R18" t="n">
-        <v>10</v>
-      </c>
       <c r="S18" t="n">
-        <v>928.5</v>
+        <v>34</v>
       </c>
       <c r="T18" t="n">
-        <v>21</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45738</v>
+        <v>45771</v>
       </c>
       <c r="B19" t="n">
-        <v>8</v>
+        <v>19.2</v>
       </c>
       <c r="C19" t="n">
-        <v>2.3</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>5</v>
+        <v>12.1</v>
       </c>
       <c r="E19" t="n">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F19" t="n">
-        <v>10.9</v>
+        <v>26.2</v>
       </c>
       <c r="G19" t="n">
-        <v>15</v>
+        <v>13.4</v>
       </c>
       <c r="H19" t="n">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="I19" t="n">
-        <v>3.3</v>
+        <v>1.7</v>
       </c>
       <c r="J19" t="n">
-        <v>13.6</v>
+        <v>5.8</v>
       </c>
       <c r="K19" t="n">
-        <v>16</v>
+        <v>4.5</v>
       </c>
       <c r="L19" t="n">
-        <v>92</v>
+        <v>943.5</v>
       </c>
       <c r="M19" t="n">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="N19" t="n">
-        <v>9.5</v>
+        <v>938.3</v>
       </c>
       <c r="O19" t="n">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="P19" t="n">
-        <v>21.1</v>
+        <v>45</v>
       </c>
       <c r="Q19" t="n">
-        <v>930.2</v>
+        <v>84</v>
       </c>
       <c r="R19" t="n">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="S19" t="n">
-        <v>927</v>
+        <v>25</v>
       </c>
       <c r="T19" t="n">
-        <v>16</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45739</v>
+        <v>45772</v>
       </c>
       <c r="B20" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>3.8</v>
+        <v>13.2</v>
       </c>
       <c r="E20" t="n">
-        <v>7</v>
+        <v>5.3</v>
       </c>
       <c r="F20" t="n">
-        <v>12.3</v>
+        <v>26.8</v>
       </c>
       <c r="G20" t="n">
-        <v>15.3</v>
+        <v>14</v>
       </c>
       <c r="H20" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I20" t="n">
-        <v>1.7</v>
+        <v>3.1</v>
       </c>
       <c r="J20" t="n">
-        <v>9.699999999999999</v>
+        <v>11.9</v>
       </c>
       <c r="K20" t="n">
-        <v>1.1</v>
+        <v>23.1</v>
       </c>
       <c r="L20" t="n">
-        <v>61</v>
+        <v>938.9</v>
       </c>
       <c r="M20" t="n">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="N20" t="n">
-        <v>2.2</v>
+        <v>935</v>
       </c>
       <c r="O20" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="P20" t="n">
-        <v>15.1</v>
+        <v>49</v>
       </c>
       <c r="Q20" t="n">
-        <v>934</v>
+        <v>78</v>
       </c>
       <c r="R20" t="n">
-        <v>24</v>
+        <v>3.1</v>
       </c>
       <c r="S20" t="n">
-        <v>928.7</v>
+        <v>27</v>
       </c>
       <c r="T20" t="n">
-        <v>4</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45740</v>
+        <v>45773</v>
       </c>
       <c r="B21" t="n">
-        <v>9.199999999999999</v>
+        <v>16.7</v>
       </c>
       <c r="C21" t="n">
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>4.3</v>
+        <v>11.8</v>
       </c>
       <c r="E21" t="n">
-        <v>7</v>
+        <v>5.2</v>
       </c>
       <c r="F21" t="n">
-        <v>14</v>
+        <v>21.6</v>
       </c>
       <c r="G21" t="n">
-        <v>14</v>
+        <v>13.4</v>
       </c>
       <c r="H21" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I21" t="n">
-        <v>3.3</v>
+        <v>1.4</v>
       </c>
       <c r="J21" t="n">
-        <v>12.5</v>
+        <v>7.8</v>
       </c>
       <c r="K21" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="L21" t="n">
+        <v>943.9</v>
+      </c>
+      <c r="M21" t="n">
+        <v>23</v>
+      </c>
+      <c r="N21" t="n">
+        <v>937.2</v>
+      </c>
+      <c r="O21" t="n">
+        <v>2</v>
+      </c>
+      <c r="P21" t="n">
+        <v>48</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>78</v>
+      </c>
+      <c r="R21" t="n">
+        <v>5</v>
+      </c>
+      <c r="S21" t="n">
+        <v>31</v>
+      </c>
+      <c r="T21" t="n">
         <v>18</v>
-      </c>
-      <c r="L21" t="n">
-        <v>70</v>
-      </c>
-      <c r="M21" t="n">
-        <v>96</v>
-      </c>
-      <c r="N21" t="n">
-        <v>23.5</v>
-      </c>
-      <c r="O21" t="n">
-        <v>45</v>
-      </c>
-      <c r="P21" t="n">
-        <v>14.2</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>941.4</v>
-      </c>
-      <c r="R21" t="n">
-        <v>24</v>
-      </c>
-      <c r="S21" t="n">
-        <v>933.7</v>
-      </c>
-      <c r="T21" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45741</v>
+        <v>45774</v>
       </c>
       <c r="B22" t="n">
-        <v>11</v>
+        <v>15.2</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
+        <v>9</v>
+      </c>
+      <c r="E22" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="F22" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="G22" t="n">
+        <v>14.4</v>
+      </c>
+      <c r="H22" t="n">
+        <v>6</v>
+      </c>
+      <c r="I22" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="J22" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="K22" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="L22" t="n">
+        <v>944.6</v>
+      </c>
+      <c r="M22" t="n">
+        <v>9</v>
+      </c>
+      <c r="N22" t="n">
+        <v>941.8</v>
+      </c>
+      <c r="O22" t="n">
+        <v>18</v>
+      </c>
+      <c r="P22" t="n">
+        <v>47</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>71</v>
+      </c>
+      <c r="R22" t="n">
         <v>6.2</v>
       </c>
-      <c r="E22" t="n">
-        <v>1</v>
-      </c>
-      <c r="F22" t="n">
-        <v>15.9</v>
-      </c>
-      <c r="G22" t="n">
-        <v>15.2</v>
-      </c>
-      <c r="H22" t="n">
-        <v>3</v>
-      </c>
-      <c r="I22" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="J22" t="n">
-        <v>9.4</v>
-      </c>
-      <c r="K22" t="n">
-        <v>11</v>
-      </c>
-      <c r="L22" t="n">
-        <v>60</v>
-      </c>
-      <c r="M22" t="n">
-        <v>97</v>
-      </c>
-      <c r="N22" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="O22" t="n">
-        <v>41</v>
-      </c>
-      <c r="P22" t="n">
-        <v>15.4</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>944.1</v>
-      </c>
-      <c r="R22" t="n">
-        <v>23</v>
-      </c>
       <c r="S22" t="n">
-        <v>941</v>
+        <v>34</v>
       </c>
       <c r="T22" t="n">
-        <v>2</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45742</v>
+        <v>45775</v>
       </c>
       <c r="B23" t="n">
-        <v>10.2</v>
+        <v>17.1</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>5.2</v>
+        <v>10.7</v>
       </c>
       <c r="E23" t="n">
-        <v>6.4</v>
+        <v>6</v>
       </c>
       <c r="F23" t="n">
-        <v>15.2</v>
+        <v>23.5</v>
       </c>
       <c r="G23" t="n">
-        <v>12.3</v>
+        <v>14</v>
       </c>
       <c r="H23" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I23" t="n">
-        <v>1.4</v>
+        <v>2.8</v>
       </c>
       <c r="J23" t="n">
-        <v>7.2</v>
+        <v>11.7</v>
       </c>
       <c r="K23" t="n">
-        <v>18.5</v>
+        <v>23</v>
       </c>
       <c r="L23" t="n">
-        <v>60</v>
+        <v>943.4</v>
       </c>
       <c r="M23" t="n">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="N23" t="n">
-        <v>6.3</v>
+        <v>938.9</v>
       </c>
       <c r="O23" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="P23" t="n">
+        <v>45</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>73</v>
+      </c>
+      <c r="R23" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="S23" t="n">
+        <v>28</v>
+      </c>
+      <c r="T23" t="n">
         <v>14.2</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>944</v>
-      </c>
-      <c r="R23" t="n">
-        <v>0</v>
-      </c>
-      <c r="S23" t="n">
-        <v>939.6</v>
-      </c>
-      <c r="T23" t="n">
-        <v>16</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45743</v>
+        <v>45776</v>
       </c>
       <c r="B24" t="n">
-        <v>10.2</v>
+        <v>17</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>4.3</v>
+        <v>11.8</v>
       </c>
       <c r="E24" t="n">
+        <v>6</v>
+      </c>
+      <c r="F24" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="G24" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="H24" t="n">
+        <v>35</v>
+      </c>
+      <c r="I24" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="J24" t="n">
+        <v>11.1</v>
+      </c>
+      <c r="K24" t="n">
+        <v>14.1</v>
+      </c>
+      <c r="L24" t="n">
+        <v>940.9</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" t="n">
+        <v>936</v>
+      </c>
+      <c r="O24" t="n">
+        <v>16</v>
+      </c>
+      <c r="P24" t="n">
+        <v>52</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>69</v>
+      </c>
+      <c r="R24" t="n">
         <v>6.4</v>
       </c>
-      <c r="F24" t="n">
-        <v>16.1</v>
-      </c>
-      <c r="G24" t="n">
-        <v>16.2</v>
-      </c>
-      <c r="H24" t="n">
-        <v>23</v>
-      </c>
-      <c r="I24" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="J24" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="K24" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="L24" t="n">
-        <v>58</v>
-      </c>
-      <c r="M24" t="n">
-        <v>85</v>
-      </c>
-      <c r="N24" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="O24" t="n">
-        <v>41</v>
-      </c>
-      <c r="P24" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>940.1</v>
-      </c>
-      <c r="R24" t="n">
-        <v>0</v>
-      </c>
       <c r="S24" t="n">
-        <v>936.4</v>
+        <v>38</v>
       </c>
       <c r="T24" t="n">
-        <v>16</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45744</v>
+        <v>45777</v>
       </c>
       <c r="B25" t="n">
-        <v>12.3</v>
+        <v>16</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>5.3</v>
       </c>
       <c r="D25" t="n">
-        <v>6.2</v>
+        <v>11.4</v>
       </c>
       <c r="E25" t="n">
-        <v>4.4</v>
+        <v>5.5</v>
       </c>
       <c r="F25" t="n">
-        <v>18.4</v>
+        <v>20.5</v>
       </c>
       <c r="G25" t="n">
-        <v>15</v>
+        <v>16.1</v>
       </c>
       <c r="H25" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I25" t="n">
-        <v>1.1</v>
+        <v>3.3</v>
       </c>
       <c r="J25" t="n">
-        <v>8.300000000000001</v>
+        <v>12.8</v>
       </c>
       <c r="K25" t="n">
-        <v>17.3</v>
+        <v>20.3</v>
       </c>
       <c r="L25" t="n">
+        <v>939</v>
+      </c>
+      <c r="M25" t="n">
+        <v>8</v>
+      </c>
+      <c r="N25" t="n">
+        <v>933.6</v>
+      </c>
+      <c r="O25" t="n">
+        <v>17</v>
+      </c>
+      <c r="P25" t="n">
+        <v>60</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>99</v>
+      </c>
+      <c r="R25" t="n">
+        <v>23.2</v>
+      </c>
+      <c r="S25" t="n">
         <v>49</v>
       </c>
-      <c r="M25" t="n">
-        <v>84</v>
-      </c>
-      <c r="N25" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="O25" t="n">
-        <v>26</v>
-      </c>
-      <c r="P25" t="n">
-        <v>14.3</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>941.8</v>
-      </c>
-      <c r="R25" t="n">
-        <v>23</v>
-      </c>
-      <c r="S25" t="n">
-        <v>937.4</v>
-      </c>
       <c r="T25" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45745</v>
+        <v>45778</v>
       </c>
       <c r="B26" t="n">
-        <v>12.8</v>
+        <v>16.7</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>22.7</v>
       </c>
       <c r="D26" t="n">
-        <v>6.2</v>
+        <v>11.7</v>
       </c>
       <c r="E26" t="n">
-        <v>5.5</v>
+        <v>0.5</v>
       </c>
       <c r="F26" t="n">
-        <v>19.3</v>
+        <v>21.7</v>
       </c>
       <c r="G26" t="n">
-        <v>14.3</v>
+        <v>16.5</v>
       </c>
       <c r="H26" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I26" t="n">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="J26" t="n">
-        <v>10.8</v>
+        <v>6.4</v>
       </c>
       <c r="K26" t="n">
-        <v>16.3</v>
+        <v>23.59</v>
       </c>
       <c r="L26" t="n">
-        <v>51</v>
+        <v>938.8</v>
       </c>
       <c r="M26" t="n">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="N26" t="n">
-        <v>6.5</v>
+        <v>934.2</v>
       </c>
       <c r="O26" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="P26" t="n">
-        <v>14.3</v>
+        <v>71</v>
       </c>
       <c r="Q26" t="n">
-        <v>943.2</v>
+        <v>95</v>
       </c>
       <c r="R26" t="n">
-        <v>10</v>
+        <v>23.59</v>
       </c>
       <c r="S26" t="n">
-        <v>940.4</v>
+        <v>67</v>
       </c>
       <c r="T26" t="n">
-        <v>17</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45746</v>
+        <v>45779</v>
       </c>
       <c r="B27" t="n">
-        <v>12.6</v>
+        <v>15</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>13.6</v>
       </c>
       <c r="D27" t="n">
-        <v>4.2</v>
+        <v>10.5</v>
       </c>
       <c r="E27" t="n">
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
       <c r="F27" t="n">
-        <v>20.9</v>
+        <v>19.5</v>
       </c>
       <c r="G27" t="n">
-        <v>16.1</v>
+        <v>14.2</v>
       </c>
       <c r="H27" t="n">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="I27" t="n">
-        <v>2.2</v>
+        <v>2.8</v>
       </c>
       <c r="J27" t="n">
-        <v>8.300000000000001</v>
+        <v>11.9</v>
       </c>
       <c r="K27" t="n">
-        <v>9.1</v>
+        <v>6.2</v>
       </c>
       <c r="L27" t="n">
-        <v>33</v>
+        <v>937.5</v>
       </c>
       <c r="M27" t="n">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="N27" t="n">
-        <v>6.4</v>
+        <v>932.7</v>
       </c>
       <c r="O27" t="n">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="P27" t="n">
-        <v>15.1</v>
+        <v>80</v>
       </c>
       <c r="Q27" t="n">
-        <v>943.6</v>
+        <v>96</v>
       </c>
       <c r="R27" t="n">
-        <v>10</v>
+        <v>1.1</v>
       </c>
       <c r="S27" t="n">
-        <v>940.8</v>
+        <v>65</v>
       </c>
       <c r="T27" t="n">
-        <v>17</v>
+        <v>13.4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45747</v>
+        <v>45780</v>
       </c>
       <c r="B28" t="n">
-        <v>16.9</v>
+        <v>15.8</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D28" t="n">
-        <v>9.1</v>
+        <v>11.2</v>
       </c>
       <c r="E28" t="n">
-        <v>6.1</v>
+        <v>3.2</v>
       </c>
       <c r="F28" t="n">
-        <v>24.7</v>
+        <v>20.4</v>
       </c>
       <c r="G28" t="n">
-        <v>14</v>
+        <v>14.4</v>
       </c>
       <c r="H28" t="n">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="I28" t="n">
-        <v>1.4</v>
+        <v>1.7</v>
       </c>
       <c r="J28" t="n">
-        <v>6.7</v>
+        <v>12.2</v>
       </c>
       <c r="K28" t="n">
-        <v>4.4</v>
+        <v>19.4</v>
       </c>
       <c r="L28" t="n">
-        <v>34</v>
+        <v>938.2</v>
       </c>
       <c r="M28" t="n">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="N28" t="n">
-        <v>6.1</v>
+        <v>935.4</v>
       </c>
       <c r="O28" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="P28" t="n">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="Q28" t="n">
-        <v>942.6</v>
+        <v>97</v>
       </c>
       <c r="R28" t="n">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="S28" t="n">
-        <v>935.4</v>
+        <v>41</v>
       </c>
       <c r="T28" t="n">
-        <v>16</v>
+        <v>16.1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45748</v>
+        <v>45781</v>
       </c>
       <c r="B29" t="n">
-        <v>16.9</v>
+        <v>14</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="D29" t="n">
-        <v>10.1</v>
+        <v>11.5</v>
       </c>
       <c r="E29" t="n">
-        <v>5.2</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="F29" t="n">
-        <v>23.7</v>
+        <v>16.6</v>
       </c>
       <c r="G29" t="n">
-        <v>14</v>
+        <v>12.3</v>
       </c>
       <c r="H29" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I29" t="n">
-        <v>1.9</v>
+        <v>2.8</v>
       </c>
       <c r="J29" t="n">
-        <v>7.2</v>
+        <v>10.8</v>
       </c>
       <c r="K29" t="n">
-        <v>15</v>
+        <v>15.4</v>
       </c>
       <c r="L29" t="n">
-        <v>42</v>
+        <v>936.7</v>
       </c>
       <c r="M29" t="n">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="N29" t="n">
-        <v>23.59</v>
+        <v>933.3</v>
       </c>
       <c r="O29" t="n">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="P29" t="n">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="Q29" t="n">
-        <v>935.4</v>
+        <v>98</v>
       </c>
       <c r="R29" t="n">
-        <v>0</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="S29" t="n">
-        <v>927.2</v>
+        <v>59</v>
       </c>
       <c r="T29" t="n">
-        <v>24</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45749</v>
+        <v>45782</v>
       </c>
       <c r="B30" t="n">
-        <v>14.6</v>
+        <v>13.8</v>
       </c>
       <c r="C30" t="n">
-        <v>21.9</v>
+        <v>19.4</v>
       </c>
       <c r="D30" t="n">
         <v>10.3</v>
       </c>
       <c r="E30" t="n">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="F30" t="n">
-        <v>18.8</v>
+        <v>17.2</v>
       </c>
       <c r="G30" t="n">
-        <v>15.1</v>
+        <v>10.1</v>
       </c>
       <c r="H30" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I30" t="n">
-        <v>2.2</v>
+        <v>1.4</v>
       </c>
       <c r="J30" t="n">
-        <v>8.300000000000001</v>
+        <v>7.8</v>
       </c>
       <c r="K30" t="n">
-        <v>23.5</v>
+        <v>22</v>
       </c>
       <c r="L30" t="n">
-        <v>67</v>
+        <v>936.1</v>
       </c>
       <c r="M30" t="n">
-        <v>95</v>
+        <v>24</v>
       </c>
       <c r="N30" t="n">
-        <v>23.5</v>
+        <v>932.5</v>
       </c>
       <c r="O30" t="n">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="P30" t="n">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="Q30" t="n">
-        <v>931.4</v>
+        <v>99</v>
       </c>
       <c r="R30" t="n">
-        <v>24</v>
+        <v>4.4</v>
       </c>
       <c r="S30" t="n">
-        <v>925.5</v>
+        <v>65</v>
       </c>
       <c r="T30" t="n">
-        <v>6</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45750</v>
+        <v>45783</v>
       </c>
       <c r="B31" t="n">
-        <v>9.5</v>
+        <v>12.8</v>
       </c>
       <c r="C31" t="n">
-        <v>20.2</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
         <v>8.300000000000001</v>
       </c>
       <c r="E31" t="n">
-        <v>7</v>
+        <v>5.4</v>
       </c>
       <c r="F31" t="n">
-        <v>10.7</v>
+        <v>17.3</v>
       </c>
       <c r="G31" t="n">
-        <v>0.1</v>
+        <v>15.2</v>
       </c>
       <c r="H31" t="n">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="I31" t="n">
-        <v>2.2</v>
+        <v>1.9</v>
       </c>
       <c r="J31" t="n">
-        <v>7.8</v>
+        <v>8.9</v>
       </c>
       <c r="K31" t="n">
-        <v>0.2</v>
+        <v>23</v>
       </c>
       <c r="L31" t="n">
-        <v>98</v>
+        <v>937.2</v>
       </c>
       <c r="M31" t="n">
-        <v>98</v>
+        <v>9</v>
       </c>
       <c r="N31" t="n">
-        <v>19.45</v>
+        <v>934.7</v>
       </c>
       <c r="O31" t="n">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="P31" t="n">
-        <v>1</v>
+        <v>52</v>
       </c>
       <c r="Q31" t="n">
-        <v>935.2</v>
+        <v>80</v>
       </c>
       <c r="R31" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="S31" t="n">
-        <v>930.9</v>
+        <v>38</v>
       </c>
       <c r="T31" t="n">
-        <v>3</v>
+        <v>16.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>